<commit_message>
Versuch Verknüpfung Registrierung & Profil mit DB -> fehlerhaft
</commit_message>
<xml_diff>
--- a/docs/toDo_Liste.xlsx
+++ b/docs/toDo_Liste.xlsx
@@ -1,28 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\BrennaTuatsGuat\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8974A514-115A-48C1-BBDB-5A80ACAE600B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3740" yWindow="0" windowWidth="20400" windowHeight="13580"/>
+    <workbookView xWindow="4680" yWindow="0" windowWidth="20400" windowHeight="13584" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="64">
   <si>
     <t>ToDo</t>
   </si>
@@ -221,9 +227,6 @@
     <t>Verlinkung in Footer</t>
   </si>
   <si>
-    <t>phpMyAdmin; Test-User &amp; Test-Scores anlegen</t>
-  </si>
-  <si>
     <t>Treffpunkt</t>
   </si>
   <si>
@@ -237,12 +240,15 @@
   </si>
   <si>
     <t>t p</t>
+  </si>
+  <si>
+    <t>Fremdschlüssel fehlt noch!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1026,30 +1032,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="61.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="18">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1070,7 +1076,7 @@
       </c>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1087,7 +1093,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1101,23 +1107,26 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
@@ -1129,7 +1138,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1149,7 +1158,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1169,7 +1178,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1186,7 +1195,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -1197,7 +1206,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="18">
+    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
@@ -1206,11 +1215,11 @@
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="G12" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1224,13 +1233,13 @@
         <v>20</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H13" s="6">
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1244,7 +1253,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1255,18 +1264,18 @@
         <v>5</v>
       </c>
       <c r="E15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" t="s">
-        <v>62</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>26</v>
       </c>
@@ -1275,7 +1284,7 @@
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1292,7 +1301,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="3" customFormat="1">
+    <row r="20" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>40</v>
       </c>
@@ -1303,7 +1312,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="3" customFormat="1">
+    <row r="21" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>41</v>
       </c>
@@ -1314,10 +1323,10 @@
         <v>42</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -1331,7 +1340,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -1342,7 +1351,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>43</v>
       </c>
@@ -1351,7 +1360,7 @@
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -1365,7 +1374,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>38</v>
       </c>
@@ -1374,7 +1383,7 @@
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -1385,7 +1394,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>46</v>
       </c>
@@ -1399,7 +1408,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>56</v>
       </c>
@@ -1408,7 +1417,7 @@
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
DB aktualisiert, Profil & Routes angepasst
</commit_message>
<xml_diff>
--- a/docs/toDo_Liste.xlsx
+++ b/docs/toDo_Liste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\BrennaTuatsGuat\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8974A514-115A-48C1-BBDB-5A80ACAE600B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764F9129-58E0-4F9A-A8DF-E6243C5366E8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="0" windowWidth="20400" windowHeight="13584" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5616" yWindow="0" windowWidth="20400" windowHeight="13584" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="65">
   <si>
     <t>ToDo</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>Fremdschlüssel fehlt noch!</t>
+  </si>
+  <si>
+    <t>index.php</t>
   </si>
 </sst>
 </file>
@@ -786,7 +789,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -838,7 +841,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1042,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1350,6 +1353,9 @@
       <c r="D23" t="s">
         <v>31</v>
       </c>
+      <c r="E23" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
@@ -1459,7 +1465,7 @@
       <formula>NOT(ISERROR(SEARCH("unerledigt",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E26 D26:D27 D29:D31 D11:D24 E3 D33:D1048576 E22 D1:D9">
+  <conditionalFormatting sqref="E26 D26:D27 D29:D31 D11:D24 E3 D33:D1048576 D1:D9 E22:E23">
     <cfRule type="containsText" dxfId="38" priority="36" operator="containsText" text="Nadine">
       <formula>NOT(ISERROR(SEARCH("Nadine",D1)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Spielfeld abgeändert, Datenbank angepasst
</commit_message>
<xml_diff>
--- a/docs/toDo_Liste.xlsx
+++ b/docs/toDo_Liste.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="25590" windowHeight="14970" activeTab="1"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="25590" windowHeight="14970"/>
   </bookViews>
   <sheets>
     <sheet name="Aufgabenverteilung" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="105">
   <si>
     <t>ToDo</t>
   </si>
@@ -365,13 +365,7 @@
     <t>Routes komplett überarbeitet</t>
   </si>
   <si>
-    <t>neue DB erstellt</t>
-  </si>
-  <si>
-    <t>neue DB verknüpft</t>
-  </si>
-  <si>
-    <t>neue DB eingerichtet</t>
+    <t>neue DB erstellt/verknüpft/eingerichtet</t>
   </si>
 </sst>
 </file>
@@ -538,97 +532,7 @@
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="60">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="51">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1103,7 +1007,7 @@
   </autoFilter>
   <tableColumns count="3">
     <tableColumn id="1" name="Person"/>
-    <tableColumn id="2" name="Aufgabe" dataDxfId="59"/>
+    <tableColumn id="2" name="Aufgabe" dataDxfId="50"/>
     <tableColumn id="3" name="Details"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1409,13 +1313,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H608"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1658,16 +1562,12 @@
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
-      <c r="C28" s="9" t="s">
-        <v>105</v>
-      </c>
+      <c r="C28" s="9"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
-      <c r="C29" s="9" t="s">
-        <v>106</v>
-      </c>
+      <c r="C29" s="9"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
@@ -3422,7 +3322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
@@ -3853,182 +3753,182 @@
     <mergeCell ref="A25:E25"/>
   </mergeCells>
   <conditionalFormatting sqref="C10:C16 C26:C27 C29:C31 C34 C41:C1048576 I11:I12 C1:C2 C18:C24 C4:C8 C36:C38">
-    <cfRule type="containsText" dxfId="58" priority="52" operator="containsText" text="unerledigt">
+    <cfRule type="containsText" dxfId="49" priority="52" operator="containsText" text="unerledigt">
       <formula>NOT(ISERROR(SEARCH("unerledigt",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="53" operator="containsText" text="erledigt">
+    <cfRule type="containsText" dxfId="48" priority="53" operator="containsText" text="erledigt">
       <formula>NOT(ISERROR(SEARCH("erledigt",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="54" operator="containsText" text="unerledigt">
+    <cfRule type="containsText" dxfId="47" priority="54" operator="containsText" text="unerledigt">
       <formula>NOT(ISERROR(SEARCH("unerledigt",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="containsText" dxfId="55" priority="49" operator="containsText" text="unerledigt">
+    <cfRule type="containsText" dxfId="46" priority="49" operator="containsText" text="unerledigt">
       <formula>NOT(ISERROR(SEARCH("unerledigt",C17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="50" operator="containsText" text="erledigt">
+    <cfRule type="containsText" dxfId="45" priority="50" operator="containsText" text="erledigt">
       <formula>NOT(ISERROR(SEARCH("erledigt",C17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="51" operator="containsText" text="unerledigt">
+    <cfRule type="containsText" dxfId="44" priority="51" operator="containsText" text="unerledigt">
       <formula>NOT(ISERROR(SEARCH("unerledigt",C17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26 D26:D27 D29:D31 E3 D33:D1048576 D1:D8 G5:G7 E19:E23 D10:D24">
-    <cfRule type="containsText" dxfId="52" priority="45" operator="containsText" text="Nadine">
+    <cfRule type="containsText" dxfId="43" priority="45" operator="containsText" text="Nadine">
       <formula>NOT(ISERROR(SEARCH("Nadine",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="46" operator="containsText" text="Jassi">
+    <cfRule type="containsText" dxfId="42" priority="46" operator="containsText" text="Jassi">
       <formula>NOT(ISERROR(SEARCH("Jassi",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="47" operator="containsText" text="Mariella">
+    <cfRule type="containsText" dxfId="41" priority="47" operator="containsText" text="Mariella">
       <formula>NOT(ISERROR(SEARCH("Mariella",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="48" operator="containsText" text="Kilian">
+    <cfRule type="containsText" dxfId="40" priority="48" operator="containsText" text="Kilian">
       <formula>NOT(ISERROR(SEARCH("Kilian",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:H3">
-    <cfRule type="containsText" dxfId="48" priority="38" operator="containsText" text="unerledigt">
+    <cfRule type="containsText" dxfId="39" priority="38" operator="containsText" text="unerledigt">
       <formula>NOT(ISERROR(SEARCH("unerledigt",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="39" operator="containsText" text="erledigt">
+    <cfRule type="containsText" dxfId="38" priority="39" operator="containsText" text="erledigt">
       <formula>NOT(ISERROR(SEARCH("erledigt",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="40" operator="containsText" text="unerledigt">
+    <cfRule type="containsText" dxfId="37" priority="40" operator="containsText" text="unerledigt">
       <formula>NOT(ISERROR(SEARCH("unerledigt",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="containsText" dxfId="45" priority="35" operator="containsText" text="unerledigt">
+    <cfRule type="containsText" dxfId="36" priority="35" operator="containsText" text="unerledigt">
       <formula>NOT(ISERROR(SEARCH("unerledigt",C25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="36" operator="containsText" text="erledigt">
+    <cfRule type="containsText" dxfId="35" priority="36" operator="containsText" text="erledigt">
       <formula>NOT(ISERROR(SEARCH("erledigt",C25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="37" operator="containsText" text="unerledigt">
+    <cfRule type="containsText" dxfId="34" priority="37" operator="containsText" text="unerledigt">
       <formula>NOT(ISERROR(SEARCH("unerledigt",C25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25">
-    <cfRule type="containsText" dxfId="42" priority="31" operator="containsText" text="Nadine">
+    <cfRule type="containsText" dxfId="33" priority="31" operator="containsText" text="Nadine">
       <formula>NOT(ISERROR(SEARCH("Nadine",D25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="32" operator="containsText" text="Jassi">
+    <cfRule type="containsText" dxfId="32" priority="32" operator="containsText" text="Jassi">
       <formula>NOT(ISERROR(SEARCH("Jassi",D25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="33" operator="containsText" text="Mariella">
+    <cfRule type="containsText" dxfId="31" priority="33" operator="containsText" text="Mariella">
       <formula>NOT(ISERROR(SEARCH("Mariella",D25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="34" operator="containsText" text="Kilian">
+    <cfRule type="containsText" dxfId="30" priority="34" operator="containsText" text="Kilian">
       <formula>NOT(ISERROR(SEARCH("Kilian",D25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="containsText" dxfId="38" priority="28" operator="containsText" text="unerledigt">
+    <cfRule type="containsText" dxfId="29" priority="28" operator="containsText" text="unerledigt">
       <formula>NOT(ISERROR(SEARCH("unerledigt",C28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="29" operator="containsText" text="erledigt">
+    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="erledigt">
       <formula>NOT(ISERROR(SEARCH("erledigt",C28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="30" operator="containsText" text="unerledigt">
+    <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="unerledigt">
       <formula>NOT(ISERROR(SEARCH("unerledigt",C28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28">
-    <cfRule type="containsText" dxfId="35" priority="24" operator="containsText" text="Nadine">
+    <cfRule type="containsText" dxfId="26" priority="24" operator="containsText" text="Nadine">
       <formula>NOT(ISERROR(SEARCH("Nadine",D28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="25" operator="containsText" text="Jassi">
+    <cfRule type="containsText" dxfId="25" priority="25" operator="containsText" text="Jassi">
       <formula>NOT(ISERROR(SEARCH("Jassi",D28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="26" operator="containsText" text="Mariella">
+    <cfRule type="containsText" dxfId="24" priority="26" operator="containsText" text="Mariella">
       <formula>NOT(ISERROR(SEARCH("Mariella",D28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="27" operator="containsText" text="Kilian">
+    <cfRule type="containsText" dxfId="23" priority="27" operator="containsText" text="Kilian">
       <formula>NOT(ISERROR(SEARCH("Kilian",D28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="containsText" dxfId="31" priority="21" operator="containsText" text="unerledigt">
+    <cfRule type="containsText" dxfId="22" priority="21" operator="containsText" text="unerledigt">
       <formula>NOT(ISERROR(SEARCH("unerledigt",C9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="22" operator="containsText" text="erledigt">
+    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="erledigt">
       <formula>NOT(ISERROR(SEARCH("erledigt",C9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="23" operator="containsText" text="unerledigt">
+    <cfRule type="containsText" dxfId="20" priority="23" operator="containsText" text="unerledigt">
       <formula>NOT(ISERROR(SEARCH("unerledigt",C9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="containsText" dxfId="28" priority="17" operator="containsText" text="Nadine">
+    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="Nadine">
       <formula>NOT(ISERROR(SEARCH("Nadine",D9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="18" operator="containsText" text="Jassi">
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Jassi">
       <formula>NOT(ISERROR(SEARCH("Jassi",D9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="19" operator="containsText" text="Mariella">
+    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="Mariella">
       <formula>NOT(ISERROR(SEARCH("Mariella",D9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="20" operator="containsText" text="Kilian">
+    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="Kilian">
       <formula>NOT(ISERROR(SEARCH("Kilian",D9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="containsText" dxfId="24" priority="14" operator="containsText" text="unerledigt">
+    <cfRule type="containsText" dxfId="15" priority="14" operator="containsText" text="unerledigt">
       <formula>NOT(ISERROR(SEARCH("unerledigt",C32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="15" operator="containsText" text="erledigt">
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="erledigt">
       <formula>NOT(ISERROR(SEARCH("erledigt",C32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="16" operator="containsText" text="unerledigt">
+    <cfRule type="containsText" dxfId="13" priority="16" operator="containsText" text="unerledigt">
       <formula>NOT(ISERROR(SEARCH("unerledigt",C32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="containsText" dxfId="21" priority="10" operator="containsText" text="Nadine">
+    <cfRule type="containsText" dxfId="12" priority="10" operator="containsText" text="Nadine">
       <formula>NOT(ISERROR(SEARCH("Nadine",D32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="11" operator="containsText" text="Jassi">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="Jassi">
       <formula>NOT(ISERROR(SEARCH("Jassi",D32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="12" operator="containsText" text="Mariella">
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="Mariella">
       <formula>NOT(ISERROR(SEARCH("Mariella",D32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="13" operator="containsText" text="Kilian">
+    <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="Kilian">
       <formula>NOT(ISERROR(SEARCH("Kilian",D32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="containsText" dxfId="17" priority="7" operator="containsText" text="unerledigt">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="unerledigt">
       <formula>NOT(ISERROR(SEARCH("unerledigt",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="8" operator="containsText" text="erledigt">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="erledigt">
       <formula>NOT(ISERROR(SEARCH("erledigt",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="unerledigt">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="unerledigt">
       <formula>NOT(ISERROR(SEARCH("unerledigt",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="unerledigt">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="unerledigt">
       <formula>NOT(ISERROR(SEARCH("unerledigt",C33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="erledigt">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="erledigt">
       <formula>NOT(ISERROR(SEARCH("erledigt",C33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="unerledigt">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="unerledigt">
       <formula>NOT(ISERROR(SEARCH("unerledigt",C33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="unerledigt">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="unerledigt">
       <formula>NOT(ISERROR(SEARCH("unerledigt",C35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="erledigt">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="erledigt">
       <formula>NOT(ISERROR(SEARCH("erledigt",C35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="unerledigt">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="unerledigt">
       <formula>NOT(ISERROR(SEARCH("unerledigt",C35)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>